<commit_message>
Manufaktur, Produksi, cetak produksi tahunan, print preview produksi tahunan
</commit_message>
<xml_diff>
--- a/Documen Aturusaha/Format Laporan/1. format laporan produksi.xlsx
+++ b/Documen Aturusaha/Format Laporan/1. format laporan produksi.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Kantor\Cloning Repo Aturusaha.com\New31SIM11\Documen Aturusaha\Format Laporan\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F29BE22-FBC1-4629-B892-63F724AFD84C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="75" windowWidth="15255" windowHeight="7905" tabRatio="786" activeTab="3"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="786" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="lap-produksi" sheetId="1" r:id="rId1"/>
@@ -17,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="96">
   <si>
     <t>Laporan Produksi</t>
   </si>
@@ -293,19 +299,38 @@
   </si>
   <si>
     <t>sum(p_tambah_produksi.jum_bdp_rusak)</t>
+  </si>
+  <si>
+    <t>Per Barang</t>
+  </si>
+  <si>
+    <t>Default Barang Kosong</t>
+  </si>
+  <si>
+    <t>Tgl Produksi</t>
+  </si>
+  <si>
+    <t>per Row</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -366,6 +391,13 @@
     <font>
       <sz val="9"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -497,139 +529,155 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -637,6 +685,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -683,7 +739,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -715,9 +771,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -749,6 +823,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -924,14 +1016,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:M39"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5.5703125" customWidth="1"/>
     <col min="2" max="2" width="12.5703125" customWidth="1"/>
@@ -948,38 +1040,38 @@
     <col min="13" max="13" width="15.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:13">
-      <c r="A2" s="25" t="s">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" s="43" t="s">
         <v>26</v>
       </c>
-      <c r="B2" s="25"/>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
-      <c r="G2" s="25"/>
-      <c r="H2" s="25"/>
-      <c r="I2" s="25"/>
-      <c r="J2" s="25"/>
-      <c r="K2" s="25"/>
-      <c r="L2" s="25"/>
-      <c r="M2" s="30"/>
-    </row>
-    <row r="3" spans="1:13" s="8" customFormat="1">
-      <c r="A3" s="31"/>
-      <c r="B3" s="31"/>
-      <c r="C3" s="31"/>
-      <c r="D3" s="31"/>
-      <c r="E3" s="31"/>
-      <c r="F3" s="31"/>
-      <c r="G3" s="31"/>
-      <c r="H3" s="31"/>
-      <c r="I3" s="31"/>
-      <c r="J3" s="31"/>
-      <c r="K3" s="31"/>
-      <c r="L3" s="31"/>
-    </row>
-    <row r="4" spans="1:13">
+      <c r="B2" s="43"/>
+      <c r="C2" s="43"/>
+      <c r="D2" s="43"/>
+      <c r="E2" s="43"/>
+      <c r="F2" s="43"/>
+      <c r="G2" s="43"/>
+      <c r="H2" s="43"/>
+      <c r="I2" s="43"/>
+      <c r="J2" s="43"/>
+      <c r="K2" s="43"/>
+      <c r="L2" s="43"/>
+      <c r="M2" s="21"/>
+    </row>
+    <row r="3" spans="1:13" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="22"/>
+      <c r="B3" s="22"/>
+      <c r="C3" s="22"/>
+      <c r="D3" s="22"/>
+      <c r="E3" s="22"/>
+      <c r="F3" s="22"/>
+      <c r="G3" s="22"/>
+      <c r="H3" s="22"/>
+      <c r="I3" s="22"/>
+      <c r="J3" s="22"/>
+      <c r="K3" s="22"/>
+      <c r="L3" s="22"/>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B4" s="7" t="s">
         <v>18</v>
       </c>
@@ -991,48 +1083,48 @@
       <c r="F4" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="L4" s="32" t="s">
+      <c r="L4" s="23" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:13">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B5" s="10"/>
       <c r="C5" s="9"/>
       <c r="D5" s="10"/>
       <c r="E5" s="9"/>
       <c r="F5" s="10"/>
-      <c r="L5" s="41"/>
-    </row>
-    <row r="6" spans="1:13">
+      <c r="L5" s="32"/>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B6" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="C6" s="39" t="s">
+      <c r="C6" s="30" t="s">
         <v>46</v>
       </c>
       <c r="D6" s="11"/>
-      <c r="E6" s="40"/>
+      <c r="E6" s="31"/>
       <c r="F6" s="11"/>
       <c r="G6" s="9"/>
       <c r="H6" s="9"/>
-      <c r="L6" s="41"/>
-    </row>
-    <row r="7" spans="1:13">
+      <c r="L6" s="32"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B7" s="10"/>
       <c r="C7" s="9"/>
       <c r="D7" s="10"/>
       <c r="E7" s="12"/>
       <c r="F7" s="10"/>
-      <c r="L7" s="41"/>
-    </row>
-    <row r="8" spans="1:13">
+      <c r="L7" s="32"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>5</v>
       </c>
       <c r="B8" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="C8" s="38" t="s">
+      <c r="C8" s="29" t="s">
         <v>47</v>
       </c>
       <c r="D8" s="10"/>
@@ -1040,96 +1132,96 @@
         <v>5</v>
       </c>
       <c r="F8" s="10"/>
-      <c r="L8" s="41"/>
-    </row>
-    <row r="9" spans="1:13" s="8" customFormat="1">
-      <c r="A9" s="28"/>
-      <c r="B9" s="28"/>
-      <c r="C9" s="28"/>
-      <c r="D9" s="28"/>
-      <c r="E9" s="28"/>
-      <c r="F9" s="28"/>
-      <c r="G9" s="28"/>
-      <c r="H9" s="28"/>
-      <c r="I9" s="28"/>
-      <c r="J9" s="28"/>
-      <c r="K9" s="28"/>
-      <c r="L9" s="28"/>
-    </row>
-    <row r="10" spans="1:13">
-      <c r="A10" s="27" t="s">
+      <c r="L8" s="32"/>
+    </row>
+    <row r="9" spans="1:13" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="46"/>
+      <c r="B9" s="46"/>
+      <c r="C9" s="46"/>
+      <c r="D9" s="46"/>
+      <c r="E9" s="46"/>
+      <c r="F9" s="46"/>
+      <c r="G9" s="46"/>
+      <c r="H9" s="46"/>
+      <c r="I9" s="46"/>
+      <c r="J9" s="46"/>
+      <c r="K9" s="46"/>
+      <c r="L9" s="46"/>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" s="45" t="s">
         <v>29</v>
       </c>
-      <c r="B10" s="27"/>
-      <c r="C10" s="27"/>
-      <c r="D10" s="27"/>
-      <c r="E10" s="27"/>
-      <c r="F10" s="27"/>
-      <c r="G10" s="27"/>
-      <c r="H10" s="27"/>
-      <c r="I10" s="27"/>
-      <c r="J10" s="27"/>
-      <c r="K10" s="27"/>
-      <c r="L10" s="27"/>
-    </row>
-    <row r="11" spans="1:13">
-      <c r="A11" s="26" t="s">
+      <c r="B10" s="45"/>
+      <c r="C10" s="45"/>
+      <c r="D10" s="45"/>
+      <c r="E10" s="45"/>
+      <c r="F10" s="45"/>
+      <c r="G10" s="45"/>
+      <c r="H10" s="45"/>
+      <c r="I10" s="45"/>
+      <c r="J10" s="45"/>
+      <c r="K10" s="45"/>
+      <c r="L10" s="45"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="B11" s="26"/>
-      <c r="C11" s="26"/>
-      <c r="D11" s="26"/>
-      <c r="E11" s="26"/>
-      <c r="F11" s="26"/>
-      <c r="G11" s="26"/>
-      <c r="H11" s="26"/>
-      <c r="I11" s="26"/>
-      <c r="J11" s="26"/>
-      <c r="K11" s="26"/>
-      <c r="L11" s="26"/>
+      <c r="B11" s="44"/>
+      <c r="C11" s="44"/>
+      <c r="D11" s="44"/>
+      <c r="E11" s="44"/>
+      <c r="F11" s="44"/>
+      <c r="G11" s="44"/>
+      <c r="H11" s="44"/>
+      <c r="I11" s="44"/>
+      <c r="J11" s="44"/>
+      <c r="K11" s="44"/>
+      <c r="L11" s="44"/>
       <c r="M11" s="14"/>
     </row>
-    <row r="12" spans="1:13" s="2" customFormat="1">
-      <c r="A12" s="29" t="s">
+    <row r="12" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="48" t="s">
         <v>1</v>
       </c>
-      <c r="B12" s="24" t="s">
+      <c r="B12" s="47" t="s">
         <v>15</v>
       </c>
-      <c r="C12" s="24"/>
-      <c r="D12" s="29" t="s">
+      <c r="C12" s="47"/>
+      <c r="D12" s="48" t="s">
         <v>9</v>
       </c>
-      <c r="E12" s="20" t="s">
+      <c r="E12" s="41" t="s">
         <v>2</v>
       </c>
-      <c r="F12" s="24" t="s">
+      <c r="F12" s="47" t="s">
         <v>3</v>
       </c>
-      <c r="G12" s="24"/>
-      <c r="H12" s="24" t="s">
+      <c r="G12" s="47"/>
+      <c r="H12" s="47" t="s">
         <v>4</v>
       </c>
-      <c r="I12" s="24"/>
-      <c r="J12" s="24" t="s">
+      <c r="I12" s="47"/>
+      <c r="J12" s="47" t="s">
         <v>10</v>
       </c>
-      <c r="K12" s="24"/>
-      <c r="L12" s="24"/>
-      <c r="M12" s="20" t="s">
+      <c r="K12" s="47"/>
+      <c r="L12" s="47"/>
+      <c r="M12" s="41" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:13" s="2" customFormat="1">
-      <c r="A13" s="29"/>
+    <row r="13" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="48"/>
       <c r="B13" s="5" t="s">
         <v>16</v>
       </c>
       <c r="C13" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D13" s="29"/>
-      <c r="E13" s="21"/>
+      <c r="D13" s="48"/>
+      <c r="E13" s="42"/>
       <c r="F13" s="17" t="s">
         <v>8</v>
       </c>
@@ -1151,197 +1243,197 @@
       <c r="L13" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="M13" s="21"/>
-    </row>
-    <row r="14" spans="1:13" ht="51">
-      <c r="A14" s="33"/>
-      <c r="B14" s="33" t="s">
+      <c r="M13" s="42"/>
+    </row>
+    <row r="14" spans="1:13" ht="51" x14ac:dyDescent="0.25">
+      <c r="A14" s="24"/>
+      <c r="B14" s="24" t="s">
         <v>33</v>
       </c>
-      <c r="C14" s="33" t="s">
+      <c r="C14" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="D14" s="33" t="s">
+      <c r="D14" s="24" t="s">
         <v>35</v>
       </c>
-      <c r="E14" s="34" t="s">
+      <c r="E14" s="25" t="s">
         <v>69</v>
       </c>
-      <c r="F14" s="34" t="s">
+      <c r="F14" s="25" t="s">
         <v>72</v>
       </c>
-      <c r="G14" s="34" t="s">
+      <c r="G14" s="25" t="s">
         <v>73</v>
       </c>
-      <c r="H14" s="34" t="s">
+      <c r="H14" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="I14" s="34" t="s">
+      <c r="I14" s="25" t="s">
         <v>38</v>
       </c>
-      <c r="J14" s="34" t="s">
+      <c r="J14" s="25" t="s">
         <v>39</v>
       </c>
-      <c r="K14" s="34" t="s">
+      <c r="K14" s="25" t="s">
         <v>36</v>
       </c>
-      <c r="L14" s="34" t="s">
+      <c r="L14" s="25" t="s">
         <v>40</v>
       </c>
-      <c r="M14" s="34" t="s">
+      <c r="M14" s="25" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="15" spans="1:13">
-      <c r="A15" s="35"/>
-      <c r="B15" s="35"/>
-      <c r="C15" s="35"/>
-      <c r="D15" s="35"/>
-      <c r="E15" s="36"/>
-      <c r="F15" s="36"/>
-      <c r="G15" s="36"/>
-      <c r="H15" s="36"/>
-      <c r="I15" s="36"/>
-      <c r="J15" s="36"/>
-      <c r="K15" s="36"/>
-      <c r="L15" s="36"/>
-      <c r="M15" s="36"/>
-    </row>
-    <row r="16" spans="1:13">
-      <c r="A16" s="35"/>
-      <c r="B16" s="37" t="s">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15" s="26"/>
+      <c r="B15" s="26"/>
+      <c r="C15" s="26"/>
+      <c r="D15" s="26"/>
+      <c r="E15" s="27"/>
+      <c r="F15" s="27"/>
+      <c r="G15" s="27"/>
+      <c r="H15" s="27"/>
+      <c r="I15" s="27"/>
+      <c r="J15" s="27"/>
+      <c r="K15" s="27"/>
+      <c r="L15" s="27"/>
+      <c r="M15" s="27"/>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A16" s="26"/>
+      <c r="B16" s="28" t="s">
         <v>45</v>
       </c>
-      <c r="C16" s="35"/>
-      <c r="D16" s="35"/>
-      <c r="E16" s="36"/>
-      <c r="F16" s="36"/>
-      <c r="G16" s="36"/>
-      <c r="H16" s="36"/>
-      <c r="I16" s="36"/>
-      <c r="J16" s="36"/>
-      <c r="K16" s="36"/>
-      <c r="L16" s="36"/>
-      <c r="M16" s="36"/>
-    </row>
-    <row r="17" spans="1:13">
-      <c r="A17" s="35"/>
-      <c r="B17" s="35"/>
-      <c r="C17" s="35"/>
-      <c r="D17" s="35"/>
-      <c r="E17" s="36"/>
-      <c r="F17" s="36"/>
-      <c r="G17" s="36"/>
-      <c r="H17" s="36"/>
-      <c r="I17" s="36"/>
-      <c r="J17" s="36"/>
-      <c r="K17" s="36"/>
-      <c r="L17" s="36"/>
-      <c r="M17" s="36"/>
-    </row>
-    <row r="18" spans="1:13" s="9" customFormat="1">
+      <c r="C16" s="26"/>
+      <c r="D16" s="26"/>
+      <c r="E16" s="27"/>
+      <c r="F16" s="27"/>
+      <c r="G16" s="27"/>
+      <c r="H16" s="27"/>
+      <c r="I16" s="27"/>
+      <c r="J16" s="27"/>
+      <c r="K16" s="27"/>
+      <c r="L16" s="27"/>
+      <c r="M16" s="27"/>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A17" s="26"/>
+      <c r="B17" s="26"/>
+      <c r="C17" s="26"/>
+      <c r="D17" s="26"/>
+      <c r="E17" s="27"/>
+      <c r="F17" s="27"/>
+      <c r="G17" s="27"/>
+      <c r="H17" s="27"/>
+      <c r="I17" s="27"/>
+      <c r="J17" s="27"/>
+      <c r="K17" s="27"/>
+      <c r="L17" s="27"/>
+      <c r="M17" s="27"/>
+    </row>
+    <row r="18" spans="1:13" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B18" s="16"/>
       <c r="C18" s="16"/>
     </row>
-    <row r="19" spans="1:13" s="9" customFormat="1">
+    <row r="19" spans="1:13" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B19" s="16"/>
       <c r="C19" s="16"/>
       <c r="J19" s="9" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:13">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="I20" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:13" s="6" customFormat="1">
+    <row r="21" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
         <v>22</v>
       </c>
       <c r="B21" s="7"/>
     </row>
-    <row r="22" spans="1:13">
-      <c r="A22" s="22" t="s">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A22" s="49" t="s">
         <v>23</v>
       </c>
-      <c r="B22" s="22"/>
-      <c r="C22" s="22"/>
-      <c r="D22" s="22"/>
-      <c r="E22" s="22"/>
-      <c r="F22" s="22"/>
-      <c r="G22" s="22"/>
-      <c r="H22" s="22"/>
-      <c r="I22" s="22"/>
-      <c r="J22" s="22"/>
-      <c r="K22" s="22"/>
-      <c r="L22" s="22"/>
-    </row>
-    <row r="23" spans="1:13">
+      <c r="B22" s="49"/>
+      <c r="C22" s="49"/>
+      <c r="D22" s="49"/>
+      <c r="E22" s="49"/>
+      <c r="F22" s="49"/>
+      <c r="G22" s="49"/>
+      <c r="H22" s="49"/>
+      <c r="I22" s="49"/>
+      <c r="J22" s="49"/>
+      <c r="K22" s="49"/>
+      <c r="L22" s="49"/>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
-      <c r="E23" s="22" t="s">
+      <c r="E23" s="49" t="s">
         <v>24</v>
       </c>
-      <c r="F23" s="22"/>
-      <c r="G23" s="22"/>
+      <c r="F23" s="49"/>
+      <c r="G23" s="49"/>
       <c r="H23" s="1"/>
       <c r="I23" s="1"/>
       <c r="J23" s="1"/>
       <c r="K23" s="1"/>
       <c r="L23" s="1"/>
     </row>
-    <row r="24" spans="1:13">
-      <c r="E24" s="22" t="s">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="E24" s="49" t="s">
         <v>25</v>
       </c>
-      <c r="F24" s="23"/>
-      <c r="G24" s="23"/>
-      <c r="H24" s="23"/>
-    </row>
-    <row r="26" spans="1:13">
-      <c r="A26" s="20" t="s">
+      <c r="F24" s="50"/>
+      <c r="G24" s="50"/>
+      <c r="H24" s="50"/>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A26" s="41" t="s">
         <v>1</v>
       </c>
-      <c r="B26" s="24" t="s">
+      <c r="B26" s="47" t="s">
         <v>15</v>
       </c>
-      <c r="C26" s="24"/>
-      <c r="D26" s="20" t="s">
+      <c r="C26" s="47"/>
+      <c r="D26" s="41" t="s">
         <v>9</v>
       </c>
-      <c r="E26" s="20" t="s">
+      <c r="E26" s="41" t="s">
         <v>2</v>
       </c>
-      <c r="F26" s="24" t="s">
+      <c r="F26" s="47" t="s">
         <v>3</v>
       </c>
-      <c r="G26" s="24"/>
-      <c r="H26" s="24" t="s">
+      <c r="G26" s="47"/>
+      <c r="H26" s="47" t="s">
         <v>4</v>
       </c>
-      <c r="I26" s="24"/>
-      <c r="J26" s="24" t="s">
+      <c r="I26" s="47"/>
+      <c r="J26" s="47" t="s">
         <v>10</v>
       </c>
-      <c r="K26" s="24"/>
-      <c r="L26" s="24"/>
-      <c r="M26" s="20" t="s">
+      <c r="K26" s="47"/>
+      <c r="L26" s="47"/>
+      <c r="M26" s="41" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="27" spans="1:13">
-      <c r="A27" s="21"/>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A27" s="42"/>
       <c r="B27" s="5" t="s">
         <v>16</v>
       </c>
       <c r="C27" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D27" s="21"/>
-      <c r="E27" s="21"/>
+      <c r="D27" s="42"/>
+      <c r="E27" s="42"/>
       <c r="F27" s="5" t="s">
         <v>6</v>
       </c>
@@ -1363,9 +1455,9 @@
       <c r="L27" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="M27" s="21"/>
-    </row>
-    <row r="28" spans="1:13">
+      <c r="M27" s="42"/>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="4"/>
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
@@ -1380,7 +1472,7 @@
       <c r="L28" s="4"/>
       <c r="M28" s="4"/>
     </row>
-    <row r="29" spans="1:13">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" s="4"/>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
@@ -1395,7 +1487,7 @@
       <c r="L29" s="4"/>
       <c r="M29" s="4"/>
     </row>
-    <row r="30" spans="1:13">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" s="4"/>
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
@@ -1412,7 +1504,7 @@
       <c r="L30" s="4"/>
       <c r="M30" s="4"/>
     </row>
-    <row r="35" spans="8:12">
+    <row r="35" spans="8:12" x14ac:dyDescent="0.25">
       <c r="H35" s="6" t="s">
         <v>30</v>
       </c>
@@ -1422,26 +1514,37 @@
         <v>27</v>
       </c>
     </row>
-    <row r="36" spans="8:12">
+    <row r="36" spans="8:12" x14ac:dyDescent="0.25">
       <c r="H36" s="6" t="s">
         <v>31</v>
       </c>
       <c r="I36" s="6"/>
       <c r="J36" s="6"/>
     </row>
-    <row r="38" spans="8:12">
-      <c r="L38" s="22" t="s">
+    <row r="38" spans="8:12" x14ac:dyDescent="0.25">
+      <c r="L38" s="49" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="39" spans="8:12">
+    <row r="39" spans="8:12" x14ac:dyDescent="0.25">
       <c r="H39" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="L39" s="22"/>
+      <c r="L39" s="49"/>
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="L38:L39"/>
+    <mergeCell ref="A22:L22"/>
+    <mergeCell ref="E23:G23"/>
+    <mergeCell ref="E24:H24"/>
+    <mergeCell ref="A26:A27"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="D26:D27"/>
+    <mergeCell ref="F26:G26"/>
+    <mergeCell ref="H26:I26"/>
+    <mergeCell ref="J26:L26"/>
+    <mergeCell ref="E26:E27"/>
     <mergeCell ref="M26:M27"/>
     <mergeCell ref="A2:L2"/>
     <mergeCell ref="A11:L11"/>
@@ -1455,17 +1558,6 @@
     <mergeCell ref="A12:A13"/>
     <mergeCell ref="D12:D13"/>
     <mergeCell ref="E12:E13"/>
-    <mergeCell ref="L38:L39"/>
-    <mergeCell ref="A22:L22"/>
-    <mergeCell ref="E23:G23"/>
-    <mergeCell ref="E24:H24"/>
-    <mergeCell ref="A26:A27"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="D26:D27"/>
-    <mergeCell ref="F26:G26"/>
-    <mergeCell ref="H26:I26"/>
-    <mergeCell ref="J26:L26"/>
-    <mergeCell ref="E26:E27"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
@@ -1473,14 +1565,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A2:K38"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K13" sqref="A13:K13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5.5703125" customWidth="1"/>
     <col min="2" max="2" width="12.5703125" customWidth="1"/>
@@ -1495,34 +1587,34 @@
     <col min="11" max="11" width="15.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:11">
-      <c r="A2" s="25" t="s">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="43" t="s">
         <v>26</v>
       </c>
-      <c r="B2" s="25"/>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
-      <c r="G2" s="25"/>
-      <c r="H2" s="25"/>
-      <c r="I2" s="25"/>
-      <c r="J2" s="25"/>
-      <c r="K2" s="30"/>
-    </row>
-    <row r="3" spans="1:11" s="8" customFormat="1">
-      <c r="A3" s="31"/>
-      <c r="B3" s="31"/>
-      <c r="C3" s="31"/>
-      <c r="D3" s="31"/>
-      <c r="E3" s="31"/>
-      <c r="F3" s="31"/>
-      <c r="G3" s="31"/>
-      <c r="H3" s="31"/>
-      <c r="I3" s="31"/>
-      <c r="J3" s="31"/>
-    </row>
-    <row r="4" spans="1:11">
+      <c r="B2" s="43"/>
+      <c r="C2" s="43"/>
+      <c r="D2" s="43"/>
+      <c r="E2" s="43"/>
+      <c r="F2" s="43"/>
+      <c r="G2" s="43"/>
+      <c r="H2" s="43"/>
+      <c r="I2" s="43"/>
+      <c r="J2" s="43"/>
+      <c r="K2" s="21"/>
+    </row>
+    <row r="3" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="22"/>
+      <c r="B3" s="22"/>
+      <c r="C3" s="22"/>
+      <c r="D3" s="22"/>
+      <c r="E3" s="22"/>
+      <c r="F3" s="22"/>
+      <c r="G3" s="22"/>
+      <c r="H3" s="22"/>
+      <c r="I3" s="22"/>
+      <c r="J3" s="22"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B4" s="7" t="s">
         <v>18</v>
       </c>
@@ -1535,113 +1627,113 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B5" s="10"/>
       <c r="C5" s="9"/>
       <c r="D5" s="10"/>
       <c r="E5" s="9"/>
       <c r="F5" s="10"/>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B6" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="C6" s="38" t="s">
+      <c r="C6" s="29" t="s">
         <v>48</v>
       </c>
       <c r="D6" s="11"/>
-      <c r="E6" s="40"/>
+      <c r="E6" s="31"/>
       <c r="F6" s="11"/>
       <c r="G6" s="9"/>
       <c r="H6" s="9"/>
     </row>
-    <row r="7" spans="1:11" ht="23.25">
+    <row r="7" spans="1:11" ht="23.25" x14ac:dyDescent="0.25">
       <c r="B7" s="10"/>
-      <c r="C7" s="42" t="s">
+      <c r="C7" s="33" t="s">
         <v>49</v>
       </c>
       <c r="D7" s="10"/>
       <c r="E7" s="12"/>
       <c r="F7" s="10"/>
     </row>
-    <row r="8" spans="1:11" s="8" customFormat="1">
-      <c r="A8" s="28"/>
-      <c r="B8" s="28"/>
-      <c r="C8" s="28"/>
-      <c r="D8" s="28"/>
-      <c r="E8" s="28"/>
-      <c r="F8" s="28"/>
-      <c r="G8" s="28"/>
-      <c r="H8" s="28"/>
-      <c r="I8" s="28"/>
-      <c r="J8" s="28"/>
-    </row>
-    <row r="9" spans="1:11">
-      <c r="A9" s="27"/>
-      <c r="B9" s="27"/>
-      <c r="C9" s="27"/>
-      <c r="D9" s="27"/>
-      <c r="E9" s="27"/>
-      <c r="F9" s="27"/>
-      <c r="G9" s="27"/>
-      <c r="H9" s="27"/>
-      <c r="I9" s="27"/>
-      <c r="J9" s="27"/>
-    </row>
-    <row r="10" spans="1:11">
-      <c r="A10" s="26" t="s">
+    <row r="8" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="46"/>
+      <c r="B8" s="46"/>
+      <c r="C8" s="46"/>
+      <c r="D8" s="46"/>
+      <c r="E8" s="46"/>
+      <c r="F8" s="46"/>
+      <c r="G8" s="46"/>
+      <c r="H8" s="46"/>
+      <c r="I8" s="46"/>
+      <c r="J8" s="46"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="45"/>
+      <c r="B9" s="45"/>
+      <c r="C9" s="45"/>
+      <c r="D9" s="45"/>
+      <c r="E9" s="45"/>
+      <c r="F9" s="45"/>
+      <c r="G9" s="45"/>
+      <c r="H9" s="45"/>
+      <c r="I9" s="45"/>
+      <c r="J9" s="45"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="44" t="s">
         <v>85</v>
       </c>
-      <c r="B10" s="26"/>
-      <c r="C10" s="26"/>
-      <c r="D10" s="26"/>
-      <c r="E10" s="26"/>
-      <c r="F10" s="26"/>
-      <c r="G10" s="26"/>
-      <c r="H10" s="26"/>
-      <c r="I10" s="26"/>
-      <c r="J10" s="26"/>
+      <c r="B10" s="44"/>
+      <c r="C10" s="44"/>
+      <c r="D10" s="44"/>
+      <c r="E10" s="44"/>
+      <c r="F10" s="44"/>
+      <c r="G10" s="44"/>
+      <c r="H10" s="44"/>
+      <c r="I10" s="44"/>
+      <c r="J10" s="44"/>
       <c r="K10" s="14"/>
     </row>
-    <row r="11" spans="1:11" s="19" customFormat="1">
-      <c r="A11" s="29" t="s">
+    <row r="11" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="48" t="s">
         <v>1</v>
       </c>
-      <c r="B11" s="24" t="s">
+      <c r="B11" s="47" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="24"/>
-      <c r="D11" s="29" t="s">
+      <c r="C11" s="47"/>
+      <c r="D11" s="48" t="s">
         <v>9</v>
       </c>
-      <c r="E11" s="20" t="s">
+      <c r="E11" s="41" t="s">
         <v>2</v>
       </c>
-      <c r="F11" s="24" t="s">
+      <c r="F11" s="47" t="s">
         <v>3</v>
       </c>
-      <c r="G11" s="24"/>
-      <c r="H11" s="24" t="s">
+      <c r="G11" s="47"/>
+      <c r="H11" s="47" t="s">
         <v>4</v>
       </c>
-      <c r="I11" s="24"/>
-      <c r="J11" s="43" t="s">
+      <c r="I11" s="47"/>
+      <c r="J11" s="51" t="s">
         <v>52</v>
       </c>
-      <c r="K11" s="20" t="s">
+      <c r="K11" s="41" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:11" s="19" customFormat="1">
-      <c r="A12" s="29"/>
+    <row r="12" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="48"/>
       <c r="B12" s="17" t="s">
         <v>16</v>
       </c>
       <c r="C12" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="D12" s="29"/>
-      <c r="E12" s="21"/>
+      <c r="D12" s="48"/>
+      <c r="E12" s="42"/>
       <c r="F12" s="17" t="s">
         <v>8</v>
       </c>
@@ -1654,175 +1746,175 @@
       <c r="I12" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="J12" s="44"/>
-      <c r="K12" s="21"/>
-    </row>
-    <row r="13" spans="1:11" ht="114.75">
-      <c r="A13" s="33"/>
-      <c r="B13" s="33" t="s">
+      <c r="J12" s="52"/>
+      <c r="K12" s="42"/>
+    </row>
+    <row r="13" spans="1:11" ht="114.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="24"/>
+      <c r="B13" s="24" t="s">
         <v>33</v>
       </c>
-      <c r="C13" s="33" t="s">
+      <c r="C13" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="D13" s="33" t="s">
+      <c r="D13" s="24" t="s">
         <v>35</v>
       </c>
-      <c r="E13" s="34" t="s">
+      <c r="E13" s="25" t="s">
         <v>69</v>
       </c>
-      <c r="F13" s="34" t="s">
+      <c r="F13" s="25" t="s">
         <v>74</v>
       </c>
-      <c r="G13" s="34" t="s">
+      <c r="G13" s="25" t="s">
         <v>75</v>
       </c>
-      <c r="H13" s="34" t="s">
+      <c r="H13" s="25" t="s">
         <v>50</v>
       </c>
-      <c r="I13" s="34" t="s">
+      <c r="I13" s="25" t="s">
         <v>51</v>
       </c>
-      <c r="J13" s="34" t="s">
+      <c r="J13" s="25" t="s">
         <v>53</v>
       </c>
-      <c r="K13" s="34" t="s">
+      <c r="K13" s="25" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="14" spans="1:11">
-      <c r="A14" s="35"/>
-      <c r="B14" s="35"/>
-      <c r="C14" s="35"/>
-      <c r="D14" s="35"/>
-      <c r="E14" s="36"/>
-      <c r="F14" s="36"/>
-      <c r="G14" s="36"/>
-      <c r="H14" s="36"/>
-      <c r="I14" s="36"/>
-      <c r="J14" s="36"/>
-      <c r="K14" s="36"/>
-    </row>
-    <row r="15" spans="1:11">
-      <c r="A15" s="35"/>
-      <c r="B15" s="37" t="s">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" s="26"/>
+      <c r="B14" s="26"/>
+      <c r="C14" s="26"/>
+      <c r="D14" s="26"/>
+      <c r="E14" s="27"/>
+      <c r="F14" s="27"/>
+      <c r="G14" s="27"/>
+      <c r="H14" s="27"/>
+      <c r="I14" s="27"/>
+      <c r="J14" s="27"/>
+      <c r="K14" s="27"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" s="26"/>
+      <c r="B15" s="28" t="s">
         <v>45</v>
       </c>
-      <c r="C15" s="35"/>
-      <c r="D15" s="35"/>
-      <c r="E15" s="36"/>
-      <c r="F15" s="36"/>
-      <c r="G15" s="36"/>
-      <c r="H15" s="36"/>
-      <c r="I15" s="36"/>
-      <c r="J15" s="36"/>
-      <c r="K15" s="36"/>
-    </row>
-    <row r="16" spans="1:11">
-      <c r="A16" s="35"/>
-      <c r="B16" s="35"/>
-      <c r="C16" s="35"/>
-      <c r="D16" s="35"/>
-      <c r="E16" s="36"/>
-      <c r="F16" s="36"/>
-      <c r="G16" s="36"/>
-      <c r="H16" s="36"/>
-      <c r="I16" s="36"/>
-      <c r="J16" s="36"/>
-      <c r="K16" s="36"/>
-    </row>
-    <row r="17" spans="1:11" s="9" customFormat="1">
+      <c r="C15" s="26"/>
+      <c r="D15" s="26"/>
+      <c r="E15" s="27"/>
+      <c r="F15" s="27"/>
+      <c r="G15" s="27"/>
+      <c r="H15" s="27"/>
+      <c r="I15" s="27"/>
+      <c r="J15" s="27"/>
+      <c r="K15" s="27"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" s="26"/>
+      <c r="B16" s="26"/>
+      <c r="C16" s="26"/>
+      <c r="D16" s="26"/>
+      <c r="E16" s="27"/>
+      <c r="F16" s="27"/>
+      <c r="G16" s="27"/>
+      <c r="H16" s="27"/>
+      <c r="I16" s="27"/>
+      <c r="J16" s="27"/>
+      <c r="K16" s="27"/>
+    </row>
+    <row r="17" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B17" s="16"/>
       <c r="C17" s="16"/>
     </row>
-    <row r="18" spans="1:11" s="9" customFormat="1">
+    <row r="18" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B18" s="16"/>
       <c r="C18" s="16"/>
     </row>
-    <row r="19" spans="1:11">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="I19" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:11" s="6" customFormat="1">
+    <row r="20" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
         <v>22</v>
       </c>
       <c r="B20" s="7"/>
     </row>
-    <row r="21" spans="1:11">
-      <c r="A21" s="22" t="s">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" s="49" t="s">
         <v>23</v>
       </c>
-      <c r="B21" s="22"/>
-      <c r="C21" s="22"/>
-      <c r="D21" s="22"/>
-      <c r="E21" s="22"/>
-      <c r="F21" s="22"/>
-      <c r="G21" s="22"/>
-      <c r="H21" s="22"/>
-      <c r="I21" s="22"/>
-      <c r="J21" s="22"/>
-    </row>
-    <row r="22" spans="1:11">
+      <c r="B21" s="49"/>
+      <c r="C21" s="49"/>
+      <c r="D21" s="49"/>
+      <c r="E21" s="49"/>
+      <c r="F21" s="49"/>
+      <c r="G21" s="49"/>
+      <c r="H21" s="49"/>
+      <c r="I21" s="49"/>
+      <c r="J21" s="49"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
-      <c r="E22" s="22" t="s">
+      <c r="E22" s="49" t="s">
         <v>24</v>
       </c>
-      <c r="F22" s="22"/>
-      <c r="G22" s="22"/>
+      <c r="F22" s="49"/>
+      <c r="G22" s="49"/>
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
       <c r="J22" s="1"/>
     </row>
-    <row r="23" spans="1:11">
-      <c r="E23" s="22" t="s">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E23" s="49" t="s">
         <v>25</v>
       </c>
-      <c r="F23" s="23"/>
-      <c r="G23" s="23"/>
-      <c r="H23" s="23"/>
-    </row>
-    <row r="25" spans="1:11">
-      <c r="A25" s="20" t="s">
+      <c r="F23" s="50"/>
+      <c r="G23" s="50"/>
+      <c r="H23" s="50"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A25" s="41" t="s">
         <v>1</v>
       </c>
-      <c r="B25" s="24" t="s">
+      <c r="B25" s="47" t="s">
         <v>15</v>
       </c>
-      <c r="C25" s="24"/>
-      <c r="D25" s="20" t="s">
+      <c r="C25" s="47"/>
+      <c r="D25" s="41" t="s">
         <v>9</v>
       </c>
-      <c r="E25" s="20" t="s">
+      <c r="E25" s="41" t="s">
         <v>2</v>
       </c>
-      <c r="F25" s="24" t="s">
+      <c r="F25" s="47" t="s">
         <v>3</v>
       </c>
-      <c r="G25" s="24"/>
-      <c r="H25" s="24" t="s">
+      <c r="G25" s="47"/>
+      <c r="H25" s="47" t="s">
         <v>4</v>
       </c>
-      <c r="I25" s="24"/>
+      <c r="I25" s="47"/>
       <c r="J25" s="17"/>
-      <c r="K25" s="20" t="s">
+      <c r="K25" s="41" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="26" spans="1:11">
-      <c r="A26" s="21"/>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A26" s="42"/>
       <c r="B26" s="17" t="s">
         <v>16</v>
       </c>
       <c r="C26" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="D26" s="21"/>
-      <c r="E26" s="21"/>
+      <c r="D26" s="42"/>
+      <c r="E26" s="42"/>
       <c r="F26" s="17" t="s">
         <v>6</v>
       </c>
@@ -1838,9 +1930,9 @@
       <c r="J26" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="K26" s="21"/>
-    </row>
-    <row r="27" spans="1:11">
+      <c r="K26" s="42"/>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="4"/>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
@@ -1853,7 +1945,7 @@
       <c r="J27" s="4"/>
       <c r="K27" s="4"/>
     </row>
-    <row r="28" spans="1:11">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="4"/>
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
@@ -1866,7 +1958,7 @@
       <c r="J28" s="4"/>
       <c r="K28" s="4"/>
     </row>
-    <row r="29" spans="1:11">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="4"/>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
@@ -1879,25 +1971,35 @@
       <c r="J29" s="4"/>
       <c r="K29" s="4"/>
     </row>
-    <row r="34" spans="8:9">
+    <row r="34" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H34" s="6" t="s">
         <v>30</v>
       </c>
       <c r="I34" s="6"/>
     </row>
-    <row r="35" spans="8:9">
+    <row r="35" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H35" s="6" t="s">
         <v>31</v>
       </c>
       <c r="I35" s="6"/>
     </row>
-    <row r="38" spans="8:9">
+    <row r="38" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H38" s="1" t="s">
         <v>32</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A8:J8"/>
+    <mergeCell ref="A9:J9"/>
+    <mergeCell ref="A10:J10"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="H11:I11"/>
     <mergeCell ref="H25:I25"/>
     <mergeCell ref="K25:K26"/>
     <mergeCell ref="J11:J12"/>
@@ -1910,16 +2012,6 @@
     <mergeCell ref="D25:D26"/>
     <mergeCell ref="E25:E26"/>
     <mergeCell ref="F25:G25"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A8:J8"/>
-    <mergeCell ref="A9:J9"/>
-    <mergeCell ref="A10:J10"/>
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="E11:E12"/>
-    <mergeCell ref="F11:G11"/>
-    <mergeCell ref="H11:I11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
@@ -1927,545 +2019,589 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:N49"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A2:O49"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12:A13"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5.5703125" customWidth="1"/>
-    <col min="2" max="2" width="12.5703125" customWidth="1"/>
-    <col min="3" max="3" width="14" customWidth="1"/>
-    <col min="4" max="4" width="13.28515625" customWidth="1"/>
-    <col min="5" max="5" width="11.5703125" customWidth="1"/>
-    <col min="6" max="6" width="14.28515625" customWidth="1"/>
-    <col min="7" max="7" width="14.7109375" customWidth="1"/>
-    <col min="8" max="8" width="18" customWidth="1"/>
-    <col min="12" max="12" width="0.85546875" customWidth="1"/>
-    <col min="13" max="14" width="9.140625" hidden="1" customWidth="1"/>
+    <col min="2" max="3" width="12.5703125" customWidth="1"/>
+    <col min="4" max="4" width="14" customWidth="1"/>
+    <col min="5" max="5" width="13.28515625" customWidth="1"/>
+    <col min="6" max="6" width="11.5703125" customWidth="1"/>
+    <col min="7" max="7" width="14.28515625" customWidth="1"/>
+    <col min="8" max="8" width="14.7109375" customWidth="1"/>
+    <col min="9" max="9" width="18" customWidth="1"/>
+    <col min="13" max="13" width="0.85546875" customWidth="1"/>
+    <col min="14" max="15" width="9.140625" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:14">
-      <c r="A2" s="25" t="s">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2" s="43" t="s">
         <v>26</v>
       </c>
-      <c r="B2" s="25"/>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
-      <c r="G2" s="25"/>
-      <c r="H2" s="30"/>
-    </row>
-    <row r="3" spans="1:14" s="8" customFormat="1">
-      <c r="A3" s="31"/>
-      <c r="B3" s="31"/>
-      <c r="C3" s="31"/>
-      <c r="D3" s="31"/>
-      <c r="E3" s="31"/>
-      <c r="F3" s="31"/>
-      <c r="G3" s="31"/>
-    </row>
-    <row r="4" spans="1:14">
+      <c r="B2" s="43"/>
+      <c r="C2" s="43"/>
+      <c r="D2" s="43"/>
+      <c r="E2" s="43"/>
+      <c r="F2" s="43"/>
+      <c r="G2" s="43"/>
+      <c r="H2" s="43"/>
+      <c r="I2" s="21"/>
+    </row>
+    <row r="3" spans="1:15" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="22"/>
+      <c r="B3" s="22"/>
+      <c r="C3" s="22"/>
+      <c r="D3" s="22"/>
+      <c r="E3" s="22"/>
+      <c r="F3" s="22"/>
+      <c r="G3" s="22"/>
+      <c r="H3" s="22"/>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B4" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="C4" s="38" t="s">
+      <c r="C4" s="7"/>
+      <c r="D4" s="29" t="s">
         <v>48</v>
       </c>
-      <c r="D4" s="13" t="s">
+      <c r="E4" s="13" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:14">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B5" s="10"/>
-      <c r="C5" s="9"/>
-      <c r="D5" s="10"/>
-    </row>
-    <row r="6" spans="1:14">
+      <c r="C5" s="10"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="10"/>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B6" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="C6" s="38" t="s">
+      <c r="C6" s="7"/>
+      <c r="D6" s="29" t="s">
         <v>48</v>
       </c>
-      <c r="D6" s="11"/>
-      <c r="E6" s="9"/>
+      <c r="E6" s="11"/>
       <c r="F6" s="9"/>
-    </row>
-    <row r="7" spans="1:14">
+      <c r="G6" s="9"/>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B7" s="10"/>
-      <c r="C7" s="40"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="9" t="s">
+      <c r="C7" s="10"/>
+      <c r="D7" s="31"/>
+      <c r="E7" s="11"/>
+      <c r="F7" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="F7" s="9"/>
-    </row>
-    <row r="8" spans="1:14">
+      <c r="G7" s="9"/>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B8" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="C8" s="38" t="s">
+      <c r="C8" s="7"/>
+      <c r="D8" s="29" t="s">
         <v>48</v>
       </c>
-      <c r="D8" s="10" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" s="8" customFormat="1">
-      <c r="A9" s="28"/>
-      <c r="B9" s="28"/>
-      <c r="C9" s="28"/>
-      <c r="D9" s="28"/>
-      <c r="E9" s="28"/>
-      <c r="F9" s="28"/>
-      <c r="G9" s="28"/>
-    </row>
-    <row r="10" spans="1:14" ht="29.25" customHeight="1">
-      <c r="A10" s="54" t="s">
+      <c r="E8" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="F8" s="56" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="46"/>
+      <c r="B9" s="46"/>
+      <c r="C9" s="46"/>
+      <c r="D9" s="46"/>
+      <c r="E9" s="46"/>
+      <c r="F9" s="46"/>
+      <c r="G9" s="46"/>
+      <c r="H9" s="46"/>
+    </row>
+    <row r="10" spans="1:15" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="55" t="s">
         <v>84</v>
       </c>
-      <c r="B10" s="54"/>
-      <c r="C10" s="54"/>
-      <c r="D10" s="54"/>
-      <c r="E10" s="54"/>
-      <c r="F10" s="54"/>
-      <c r="G10" s="54"/>
-      <c r="H10" s="54"/>
-      <c r="I10" s="54"/>
-      <c r="J10" s="54"/>
-      <c r="K10" s="54"/>
-      <c r="L10" s="54"/>
-      <c r="M10" s="54"/>
-      <c r="N10" s="54"/>
-    </row>
-    <row r="11" spans="1:14">
-      <c r="A11" s="26" t="s">
+      <c r="B10" s="55"/>
+      <c r="C10" s="55"/>
+      <c r="D10" s="55"/>
+      <c r="E10" s="55"/>
+      <c r="F10" s="55"/>
+      <c r="G10" s="55"/>
+      <c r="H10" s="55"/>
+      <c r="I10" s="55"/>
+      <c r="J10" s="55"/>
+      <c r="K10" s="55"/>
+      <c r="L10" s="55"/>
+      <c r="M10" s="55"/>
+      <c r="N10" s="55"/>
+      <c r="O10" s="55"/>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A11" s="44" t="s">
         <v>86</v>
       </c>
-      <c r="B11" s="26"/>
-      <c r="C11" s="26"/>
-      <c r="D11" s="26"/>
-      <c r="E11" s="26"/>
-      <c r="F11" s="26"/>
-      <c r="G11" s="26"/>
-      <c r="H11" s="14"/>
-    </row>
-    <row r="12" spans="1:14" s="19" customFormat="1" ht="15" customHeight="1">
-      <c r="A12" s="29" t="s">
+      <c r="B11" s="44"/>
+      <c r="C11" s="44"/>
+      <c r="D11" s="44"/>
+      <c r="E11" s="44"/>
+      <c r="F11" s="44"/>
+      <c r="G11" s="44"/>
+      <c r="H11" s="44"/>
+      <c r="I11" s="14"/>
+    </row>
+    <row r="12" spans="1:15" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="48" t="s">
         <v>1</v>
       </c>
-      <c r="B12" s="20" t="s">
+      <c r="B12" s="41" t="s">
         <v>55</v>
       </c>
-      <c r="C12" s="20" t="s">
+      <c r="C12" s="41" t="s">
+        <v>94</v>
+      </c>
+      <c r="D12" s="41" t="s">
         <v>2</v>
       </c>
-      <c r="D12" s="24" t="s">
+      <c r="E12" s="47" t="s">
         <v>3</v>
       </c>
-      <c r="E12" s="24"/>
-      <c r="F12" s="24" t="s">
+      <c r="F12" s="47"/>
+      <c r="G12" s="47" t="s">
         <v>4</v>
       </c>
-      <c r="G12" s="24"/>
-      <c r="H12" s="20" t="s">
+      <c r="H12" s="47"/>
+      <c r="I12" s="41" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:14" s="19" customFormat="1">
-      <c r="A13" s="29"/>
-      <c r="B13" s="21"/>
-      <c r="C13" s="21"/>
-      <c r="D13" s="17" t="s">
+    <row r="13" spans="1:15" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="48"/>
+      <c r="B13" s="42"/>
+      <c r="C13" s="42"/>
+      <c r="D13" s="42"/>
+      <c r="E13" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="E13" s="17" t="s">
+      <c r="F13" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="F13" s="17" t="s">
+      <c r="G13" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="G13" s="17" t="s">
+      <c r="H13" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="H13" s="21"/>
-    </row>
-    <row r="14" spans="1:14" s="19" customFormat="1" ht="102">
+      <c r="I13" s="42"/>
+    </row>
+    <row r="14" spans="1:15" s="19" customFormat="1" ht="84" x14ac:dyDescent="0.25">
       <c r="A14" s="18">
         <v>1</v>
       </c>
-      <c r="B14" s="48" t="s">
+      <c r="B14" s="37" t="s">
         <v>59</v>
       </c>
-      <c r="C14" s="49" t="s">
+      <c r="C14" s="60" t="s">
+        <v>95</v>
+      </c>
+      <c r="D14" s="38" t="s">
         <v>70</v>
       </c>
-      <c r="D14" s="50" t="s">
+      <c r="E14" s="39" t="s">
         <v>76</v>
       </c>
-      <c r="E14" s="50" t="s">
+      <c r="F14" s="39" t="s">
         <v>77</v>
       </c>
-      <c r="F14" s="34" t="s">
+      <c r="G14" s="25" t="s">
         <v>71</v>
       </c>
-      <c r="G14" s="34" t="s">
+      <c r="H14" s="25" t="s">
         <v>78</v>
       </c>
-      <c r="H14" s="15"/>
-      <c r="J14" s="19" t="s">
+      <c r="I14" s="15"/>
+      <c r="K14" s="19" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:14" s="19" customFormat="1">
+    <row r="15" spans="1:15" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="18">
         <v>2</v>
       </c>
-      <c r="B15" s="46" t="s">
+      <c r="B15" s="35" t="s">
         <v>57</v>
       </c>
-      <c r="C15" s="15"/>
-      <c r="D15" s="17"/>
+      <c r="C15" s="35"/>
+      <c r="D15" s="15"/>
       <c r="E15" s="17"/>
       <c r="F15" s="17"/>
       <c r="G15" s="17"/>
-      <c r="H15" s="15"/>
-    </row>
-    <row r="16" spans="1:14" s="19" customFormat="1">
+      <c r="H15" s="17"/>
+      <c r="I15" s="15"/>
+    </row>
+    <row r="16" spans="1:15" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="18">
         <v>3</v>
       </c>
-      <c r="B16" s="46" t="s">
+      <c r="B16" s="35" t="s">
         <v>58</v>
       </c>
-      <c r="C16" s="15"/>
-      <c r="D16" s="17"/>
+      <c r="C16" s="35"/>
+      <c r="D16" s="15"/>
       <c r="E16" s="17"/>
       <c r="F16" s="17"/>
       <c r="G16" s="17"/>
-      <c r="H16" s="15"/>
-    </row>
-    <row r="17" spans="1:8" s="19" customFormat="1">
+      <c r="H16" s="17"/>
+      <c r="I16" s="15"/>
+    </row>
+    <row r="17" spans="1:9" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="18">
         <v>4</v>
       </c>
-      <c r="B17" s="47" t="s">
+      <c r="B17" s="36" t="s">
         <v>60</v>
       </c>
-      <c r="C17" s="15"/>
-      <c r="D17" s="17"/>
+      <c r="C17" s="36"/>
+      <c r="D17" s="15"/>
       <c r="E17" s="17"/>
       <c r="F17" s="17"/>
       <c r="G17" s="17"/>
-      <c r="H17" s="15"/>
-    </row>
-    <row r="18" spans="1:8" s="19" customFormat="1">
+      <c r="H17" s="17"/>
+      <c r="I17" s="15"/>
+    </row>
+    <row r="18" spans="1:9" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="18">
         <v>5</v>
       </c>
-      <c r="B18" s="47" t="s">
+      <c r="B18" s="36" t="s">
         <v>61</v>
       </c>
-      <c r="C18" s="15"/>
-      <c r="D18" s="17"/>
+      <c r="C18" s="36"/>
+      <c r="D18" s="15"/>
       <c r="E18" s="17"/>
       <c r="F18" s="17"/>
       <c r="G18" s="17"/>
-      <c r="H18" s="15"/>
-    </row>
-    <row r="19" spans="1:8" s="19" customFormat="1">
+      <c r="H18" s="17"/>
+      <c r="I18" s="15"/>
+    </row>
+    <row r="19" spans="1:9" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="18">
         <v>6</v>
       </c>
-      <c r="B19" s="47" t="s">
+      <c r="B19" s="36" t="s">
         <v>62</v>
       </c>
-      <c r="C19" s="15"/>
-      <c r="D19" s="17"/>
+      <c r="C19" s="36"/>
+      <c r="D19" s="15"/>
       <c r="E19" s="17"/>
       <c r="F19" s="17"/>
       <c r="G19" s="17"/>
-      <c r="H19" s="15"/>
-    </row>
-    <row r="20" spans="1:8" s="19" customFormat="1">
+      <c r="H19" s="17"/>
+      <c r="I19" s="15"/>
+    </row>
+    <row r="20" spans="1:9" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="18">
         <v>7</v>
       </c>
-      <c r="B20" s="47" t="s">
+      <c r="B20" s="36" t="s">
         <v>63</v>
       </c>
-      <c r="C20" s="15"/>
-      <c r="D20" s="17"/>
+      <c r="C20" s="36"/>
+      <c r="D20" s="15"/>
       <c r="E20" s="17"/>
       <c r="F20" s="17"/>
       <c r="G20" s="17"/>
-      <c r="H20" s="15"/>
-    </row>
-    <row r="21" spans="1:8" s="19" customFormat="1">
+      <c r="H20" s="17"/>
+      <c r="I20" s="15"/>
+    </row>
+    <row r="21" spans="1:9" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="18">
         <v>8</v>
       </c>
-      <c r="B21" s="47" t="s">
+      <c r="B21" s="36" t="s">
         <v>64</v>
       </c>
-      <c r="C21" s="15"/>
-      <c r="D21" s="17"/>
+      <c r="C21" s="36"/>
+      <c r="D21" s="15"/>
       <c r="E21" s="17"/>
       <c r="F21" s="17"/>
       <c r="G21" s="17"/>
-      <c r="H21" s="15"/>
-    </row>
-    <row r="22" spans="1:8" s="19" customFormat="1">
+      <c r="H21" s="17"/>
+      <c r="I21" s="15"/>
+    </row>
+    <row r="22" spans="1:9" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="18">
         <v>9</v>
       </c>
-      <c r="B22" s="47" t="s">
+      <c r="B22" s="36" t="s">
         <v>65</v>
       </c>
-      <c r="C22" s="15"/>
-      <c r="D22" s="17"/>
+      <c r="C22" s="36"/>
+      <c r="D22" s="15"/>
       <c r="E22" s="17"/>
       <c r="F22" s="17"/>
       <c r="G22" s="17"/>
-      <c r="H22" s="15"/>
-    </row>
-    <row r="23" spans="1:8" s="19" customFormat="1">
+      <c r="H22" s="17"/>
+      <c r="I22" s="15"/>
+    </row>
+    <row r="23" spans="1:9" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="18">
         <v>10</v>
       </c>
-      <c r="B23" s="47" t="s">
+      <c r="B23" s="36" t="s">
         <v>66</v>
       </c>
-      <c r="C23" s="15"/>
-      <c r="D23" s="17"/>
+      <c r="C23" s="36"/>
+      <c r="D23" s="15"/>
       <c r="E23" s="17"/>
       <c r="F23" s="17"/>
       <c r="G23" s="17"/>
-      <c r="H23" s="15"/>
-    </row>
-    <row r="24" spans="1:8" s="19" customFormat="1">
+      <c r="H23" s="17"/>
+      <c r="I23" s="15"/>
+    </row>
+    <row r="24" spans="1:9" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="18">
         <v>11</v>
       </c>
-      <c r="B24" s="47" t="s">
+      <c r="B24" s="36" t="s">
         <v>67</v>
       </c>
-      <c r="C24" s="15"/>
-      <c r="D24" s="17"/>
+      <c r="C24" s="36"/>
+      <c r="D24" s="15"/>
       <c r="E24" s="17"/>
       <c r="F24" s="17"/>
       <c r="G24" s="17"/>
-      <c r="H24" s="15"/>
-    </row>
-    <row r="25" spans="1:8" s="19" customFormat="1">
+      <c r="H24" s="17"/>
+      <c r="I24" s="15"/>
+    </row>
+    <row r="25" spans="1:9" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="18">
         <v>12</v>
       </c>
-      <c r="B25" s="47" t="s">
+      <c r="B25" s="36" t="s">
         <v>68</v>
       </c>
-      <c r="C25" s="53"/>
-      <c r="D25" s="17"/>
+      <c r="C25" s="57"/>
+      <c r="D25" s="40"/>
       <c r="E25" s="17"/>
       <c r="F25" s="17"/>
       <c r="G25" s="17"/>
-      <c r="H25" s="15"/>
-    </row>
-    <row r="26" spans="1:8">
-      <c r="A26" s="51" t="s">
+      <c r="H25" s="17"/>
+      <c r="I25" s="15"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" s="53" t="s">
         <v>79</v>
       </c>
-      <c r="B26" s="52"/>
-      <c r="C26" s="52"/>
-      <c r="D26" s="45" t="s">
+      <c r="B26" s="54"/>
+      <c r="C26" s="54"/>
+      <c r="D26" s="54"/>
+      <c r="E26" s="34" t="s">
         <v>80</v>
       </c>
-      <c r="E26" s="45" t="s">
+      <c r="F26" s="34" t="s">
         <v>81</v>
       </c>
-      <c r="F26" s="45" t="s">
+      <c r="G26" s="34" t="s">
         <v>82</v>
       </c>
-      <c r="G26" s="45" t="s">
+      <c r="H26" s="34" t="s">
         <v>83</v>
       </c>
-      <c r="H26" s="34"/>
-    </row>
-    <row r="27" spans="1:8">
-      <c r="A27" s="35"/>
-      <c r="B27" s="35"/>
-      <c r="C27" s="36"/>
-      <c r="D27" s="36"/>
-      <c r="E27" s="36"/>
-      <c r="F27" s="36"/>
-      <c r="G27" s="36"/>
-      <c r="H27" s="36"/>
-    </row>
-    <row r="28" spans="1:8" s="9" customFormat="1">
+      <c r="I26" s="25"/>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" s="26"/>
+      <c r="B27" s="26"/>
+      <c r="C27" s="26"/>
+      <c r="D27" s="27"/>
+      <c r="E27" s="27"/>
+      <c r="F27" s="27"/>
+      <c r="G27" s="27"/>
+      <c r="H27" s="27"/>
+      <c r="I27" s="27"/>
+    </row>
+    <row r="28" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B28" s="16"/>
-      <c r="D28" s="9" t="s">
+      <c r="C28" s="20"/>
+      <c r="E28" s="9" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:8" s="9" customFormat="1">
+    <row r="29" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B29" s="16"/>
-    </row>
-    <row r="30" spans="1:8">
-      <c r="G30" t="s">
+      <c r="C29" s="20"/>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H30" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="31" spans="1:8" s="6" customFormat="1">
+    <row r="31" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="7" t="s">
         <v>22</v>
       </c>
       <c r="B31" s="7"/>
-    </row>
-    <row r="32" spans="1:8">
-      <c r="A32" s="22" t="s">
+      <c r="C31" s="7"/>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32" s="49" t="s">
         <v>23</v>
       </c>
-      <c r="B32" s="22"/>
-      <c r="C32" s="22"/>
-      <c r="D32" s="22"/>
-      <c r="E32" s="22"/>
-      <c r="F32" s="22"/>
-      <c r="G32" s="22"/>
-    </row>
-    <row r="33" spans="1:8">
+      <c r="B32" s="49"/>
+      <c r="C32" s="49"/>
+      <c r="D32" s="49"/>
+      <c r="E32" s="49"/>
+      <c r="F32" s="49"/>
+      <c r="G32" s="49"/>
+      <c r="H32" s="49"/>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
-      <c r="C33" s="22" t="s">
+      <c r="C33" s="1"/>
+      <c r="D33" s="49" t="s">
         <v>24</v>
       </c>
-      <c r="D33" s="22"/>
-      <c r="E33" s="22"/>
-      <c r="F33" s="1"/>
+      <c r="E33" s="49"/>
+      <c r="F33" s="49"/>
       <c r="G33" s="1"/>
-    </row>
-    <row r="34" spans="1:8">
-      <c r="C34" s="22" t="s">
+      <c r="H33" s="1"/>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D34" s="49" t="s">
         <v>25</v>
       </c>
-      <c r="D34" s="23"/>
-      <c r="E34" s="23"/>
-      <c r="F34" s="23"/>
-    </row>
-    <row r="36" spans="1:8">
-      <c r="A36" s="20" t="s">
+      <c r="E34" s="50"/>
+      <c r="F34" s="50"/>
+      <c r="G34" s="50"/>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A36" s="41" t="s">
         <v>1</v>
       </c>
       <c r="B36" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="C36" s="20" t="s">
+      <c r="C36" s="58"/>
+      <c r="D36" s="41" t="s">
         <v>2</v>
       </c>
-      <c r="D36" s="24" t="s">
+      <c r="E36" s="47" t="s">
         <v>3</v>
       </c>
-      <c r="E36" s="24"/>
-      <c r="F36" s="24" t="s">
+      <c r="F36" s="47"/>
+      <c r="G36" s="47" t="s">
         <v>4</v>
       </c>
-      <c r="G36" s="24"/>
-      <c r="H36" s="20" t="s">
+      <c r="H36" s="47"/>
+      <c r="I36" s="41" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="37" spans="1:8">
-      <c r="A37" s="21"/>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A37" s="42"/>
       <c r="B37" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="C37" s="21"/>
-      <c r="D37" s="17" t="s">
+      <c r="C37" s="59"/>
+      <c r="D37" s="42"/>
+      <c r="E37" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="E37" s="17" t="s">
+      <c r="F37" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="F37" s="17" t="s">
+      <c r="G37" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="G37" s="17" t="s">
+      <c r="H37" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="H37" s="21"/>
-    </row>
-    <row r="38" spans="1:8">
+      <c r="I37" s="42"/>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="4"/>
       <c r="B38" s="3"/>
-      <c r="C38" s="4"/>
+      <c r="C38" s="3"/>
       <c r="D38" s="4"/>
       <c r="E38" s="4"/>
       <c r="F38" s="4"/>
       <c r="G38" s="4"/>
       <c r="H38" s="4"/>
-    </row>
-    <row r="39" spans="1:8">
+      <c r="I38" s="4"/>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="4"/>
       <c r="B39" s="3"/>
-      <c r="C39" s="4"/>
+      <c r="C39" s="3"/>
       <c r="D39" s="4"/>
       <c r="E39" s="4"/>
       <c r="F39" s="4"/>
       <c r="G39" s="4"/>
       <c r="H39" s="4"/>
-    </row>
-    <row r="40" spans="1:8">
+      <c r="I39" s="4"/>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="4"/>
       <c r="B40" s="3"/>
-      <c r="C40" s="4"/>
+      <c r="C40" s="3"/>
       <c r="D40" s="4"/>
       <c r="E40" s="4"/>
       <c r="F40" s="4"/>
       <c r="G40" s="4"/>
       <c r="H40" s="4"/>
-    </row>
-    <row r="45" spans="1:8">
-      <c r="F45" s="6" t="s">
+      <c r="I40" s="4"/>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G45" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="G45" s="6"/>
-    </row>
-    <row r="46" spans="1:8">
-      <c r="F46" s="6" t="s">
+      <c r="H45" s="6"/>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G46" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="G46" s="6"/>
-    </row>
-    <row r="49" spans="6:6">
-      <c r="F49" s="1" t="s">
+      <c r="H46" s="6"/>
+    </row>
+    <row r="49" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G49" s="1" t="s">
         <v>32</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="19">
-    <mergeCell ref="F36:G36"/>
-    <mergeCell ref="H36:H37"/>
+  <mergeCells count="20">
+    <mergeCell ref="A2:H2"/>
+    <mergeCell ref="A9:H9"/>
+    <mergeCell ref="A11:H11"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="G36:H36"/>
+    <mergeCell ref="I36:I37"/>
     <mergeCell ref="B12:B13"/>
-    <mergeCell ref="A26:C26"/>
-    <mergeCell ref="A10:N10"/>
-    <mergeCell ref="H12:H13"/>
-    <mergeCell ref="A32:G32"/>
-    <mergeCell ref="C33:E33"/>
-    <mergeCell ref="C34:F34"/>
+    <mergeCell ref="A26:D26"/>
+    <mergeCell ref="A10:O10"/>
+    <mergeCell ref="I12:I13"/>
+    <mergeCell ref="A32:H32"/>
+    <mergeCell ref="D33:F33"/>
+    <mergeCell ref="D34:G34"/>
     <mergeCell ref="A36:A37"/>
-    <mergeCell ref="C36:C37"/>
-    <mergeCell ref="D36:E36"/>
-    <mergeCell ref="A2:G2"/>
-    <mergeCell ref="A9:G9"/>
-    <mergeCell ref="A11:G11"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="D36:D37"/>
+    <mergeCell ref="E36:F36"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
@@ -2473,14 +2609,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:N49"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A2:M49"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+    <sheetView topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5.5703125" customWidth="1"/>
     <col min="2" max="2" width="12.5703125" customWidth="1"/>
@@ -2493,133 +2629,133 @@
     <col min="12" max="13" width="9.140625" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:13">
-      <c r="A2" s="25" t="s">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" s="43" t="s">
         <v>26</v>
       </c>
-      <c r="B2" s="25"/>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
-      <c r="G2" s="25"/>
-    </row>
-    <row r="3" spans="1:13" s="8" customFormat="1">
-      <c r="A3" s="31"/>
-      <c r="B3" s="31"/>
-      <c r="C3" s="31"/>
-      <c r="D3" s="31"/>
-      <c r="E3" s="31"/>
-      <c r="F3" s="31"/>
-      <c r="G3" s="31"/>
-    </row>
-    <row r="4" spans="1:13">
+      <c r="B2" s="43"/>
+      <c r="C2" s="43"/>
+      <c r="D2" s="43"/>
+      <c r="E2" s="43"/>
+      <c r="F2" s="43"/>
+      <c r="G2" s="43"/>
+    </row>
+    <row r="3" spans="1:13" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="22"/>
+      <c r="B3" s="22"/>
+      <c r="C3" s="22"/>
+      <c r="D3" s="22"/>
+      <c r="E3" s="22"/>
+      <c r="F3" s="22"/>
+      <c r="G3" s="22"/>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B4" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="C4" s="38" t="s">
+      <c r="C4" s="29" t="s">
         <v>48</v>
       </c>
       <c r="D4" s="13" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:13">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B5" s="10"/>
       <c r="C5" s="9"/>
       <c r="D5" s="10"/>
     </row>
-    <row r="6" spans="1:13">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B6" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="C6" s="38" t="s">
+      <c r="C6" s="29" t="s">
         <v>48</v>
       </c>
       <c r="D6" s="11"/>
       <c r="E6" s="9"/>
       <c r="F6" s="9"/>
     </row>
-    <row r="7" spans="1:13">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B7" s="10"/>
-      <c r="C7" s="40"/>
+      <c r="C7" s="31"/>
       <c r="D7" s="11"/>
       <c r="E7" s="9" t="s">
         <v>5</v>
       </c>
       <c r="F7" s="9"/>
     </row>
-    <row r="8" spans="1:13">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B8" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="C8" s="38" t="s">
+      <c r="C8" s="29" t="s">
         <v>48</v>
       </c>
       <c r="D8" s="10" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:13" s="8" customFormat="1">
-      <c r="A9" s="28"/>
-      <c r="B9" s="28"/>
-      <c r="C9" s="28"/>
-      <c r="D9" s="28"/>
-      <c r="E9" s="28"/>
-      <c r="F9" s="28"/>
-      <c r="G9" s="28"/>
-    </row>
-    <row r="10" spans="1:13" ht="29.25" customHeight="1">
-      <c r="A10" s="54" t="s">
+    <row r="9" spans="1:13" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="46"/>
+      <c r="B9" s="46"/>
+      <c r="C9" s="46"/>
+      <c r="D9" s="46"/>
+      <c r="E9" s="46"/>
+      <c r="F9" s="46"/>
+      <c r="G9" s="46"/>
+    </row>
+    <row r="10" spans="1:13" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="55" t="s">
         <v>87</v>
       </c>
-      <c r="B10" s="54"/>
-      <c r="C10" s="54"/>
-      <c r="D10" s="54"/>
-      <c r="E10" s="54"/>
-      <c r="F10" s="54"/>
-      <c r="G10" s="54"/>
-      <c r="H10" s="54"/>
-      <c r="I10" s="54"/>
-      <c r="J10" s="54"/>
-      <c r="K10" s="54"/>
-      <c r="L10" s="54"/>
-      <c r="M10" s="54"/>
-    </row>
-    <row r="11" spans="1:13">
-      <c r="A11" s="26" t="s">
+      <c r="B10" s="55"/>
+      <c r="C10" s="55"/>
+      <c r="D10" s="55"/>
+      <c r="E10" s="55"/>
+      <c r="F10" s="55"/>
+      <c r="G10" s="55"/>
+      <c r="H10" s="55"/>
+      <c r="I10" s="55"/>
+      <c r="J10" s="55"/>
+      <c r="K10" s="55"/>
+      <c r="L10" s="55"/>
+      <c r="M10" s="55"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11" s="44" t="s">
         <v>56</v>
       </c>
-      <c r="B11" s="26"/>
-      <c r="C11" s="26"/>
-      <c r="D11" s="26"/>
-      <c r="E11" s="26"/>
-      <c r="F11" s="26"/>
-      <c r="G11" s="26"/>
-    </row>
-    <row r="12" spans="1:13" s="19" customFormat="1" ht="15" customHeight="1">
-      <c r="A12" s="29" t="s">
+      <c r="B11" s="44"/>
+      <c r="C11" s="44"/>
+      <c r="D11" s="44"/>
+      <c r="E11" s="44"/>
+      <c r="F11" s="44"/>
+      <c r="G11" s="44"/>
+    </row>
+    <row r="12" spans="1:13" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="48" t="s">
         <v>1</v>
       </c>
-      <c r="B12" s="20" t="s">
+      <c r="B12" s="41" t="s">
         <v>55</v>
       </c>
-      <c r="C12" s="20" t="s">
+      <c r="C12" s="41" t="s">
         <v>2</v>
       </c>
-      <c r="D12" s="24" t="s">
+      <c r="D12" s="47" t="s">
         <v>3</v>
       </c>
-      <c r="E12" s="24"/>
-      <c r="F12" s="24" t="s">
+      <c r="E12" s="47"/>
+      <c r="F12" s="47" t="s">
         <v>4</v>
       </c>
-      <c r="G12" s="24"/>
-    </row>
-    <row r="13" spans="1:13" s="19" customFormat="1">
-      <c r="A13" s="29"/>
-      <c r="B13" s="21"/>
-      <c r="C13" s="21"/>
+      <c r="G12" s="47"/>
+    </row>
+    <row r="13" spans="1:13" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="48"/>
+      <c r="B13" s="42"/>
+      <c r="C13" s="42"/>
       <c r="D13" s="17" t="s">
         <v>8</v>
       </c>
@@ -2633,37 +2769,37 @@
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:13" s="19" customFormat="1" ht="84">
+    <row r="14" spans="1:13" s="19" customFormat="1" ht="84" x14ac:dyDescent="0.25">
       <c r="A14" s="18">
         <v>1</v>
       </c>
-      <c r="B14" s="48" t="s">
+      <c r="B14" s="37" t="s">
         <v>59</v>
       </c>
-      <c r="C14" s="49" t="s">
+      <c r="C14" s="38" t="s">
         <v>70</v>
       </c>
-      <c r="D14" s="50" t="s">
+      <c r="D14" s="39" t="s">
         <v>88</v>
       </c>
-      <c r="E14" s="50" t="s">
+      <c r="E14" s="39" t="s">
         <v>89</v>
       </c>
-      <c r="F14" s="34" t="s">
+      <c r="F14" s="25" t="s">
         <v>90</v>
       </c>
-      <c r="G14" s="34" t="s">
+      <c r="G14" s="25" t="s">
         <v>91</v>
       </c>
       <c r="I14" s="19" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:13" s="19" customFormat="1">
+    <row r="15" spans="1:13" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="18">
         <v>2</v>
       </c>
-      <c r="B15" s="46" t="s">
+      <c r="B15" s="35" t="s">
         <v>57</v>
       </c>
       <c r="C15" s="15"/>
@@ -2672,11 +2808,11 @@
       <c r="F15" s="17"/>
       <c r="G15" s="17"/>
     </row>
-    <row r="16" spans="1:13" s="19" customFormat="1">
+    <row r="16" spans="1:13" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="18">
         <v>3</v>
       </c>
-      <c r="B16" s="46" t="s">
+      <c r="B16" s="35" t="s">
         <v>58</v>
       </c>
       <c r="C16" s="15"/>
@@ -2685,11 +2821,11 @@
       <c r="F16" s="17"/>
       <c r="G16" s="17"/>
     </row>
-    <row r="17" spans="1:7" s="19" customFormat="1">
+    <row r="17" spans="1:7" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="18">
         <v>4</v>
       </c>
-      <c r="B17" s="47" t="s">
+      <c r="B17" s="36" t="s">
         <v>60</v>
       </c>
       <c r="C17" s="15"/>
@@ -2698,11 +2834,11 @@
       <c r="F17" s="17"/>
       <c r="G17" s="17"/>
     </row>
-    <row r="18" spans="1:7" s="19" customFormat="1">
+    <row r="18" spans="1:7" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="18">
         <v>5</v>
       </c>
-      <c r="B18" s="47" t="s">
+      <c r="B18" s="36" t="s">
         <v>61</v>
       </c>
       <c r="C18" s="15"/>
@@ -2711,11 +2847,11 @@
       <c r="F18" s="17"/>
       <c r="G18" s="17"/>
     </row>
-    <row r="19" spans="1:7" s="19" customFormat="1">
+    <row r="19" spans="1:7" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="18">
         <v>6</v>
       </c>
-      <c r="B19" s="47" t="s">
+      <c r="B19" s="36" t="s">
         <v>62</v>
       </c>
       <c r="C19" s="15"/>
@@ -2724,11 +2860,11 @@
       <c r="F19" s="17"/>
       <c r="G19" s="17"/>
     </row>
-    <row r="20" spans="1:7" s="19" customFormat="1">
+    <row r="20" spans="1:7" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="18">
         <v>7</v>
       </c>
-      <c r="B20" s="47" t="s">
+      <c r="B20" s="36" t="s">
         <v>63</v>
       </c>
       <c r="C20" s="15"/>
@@ -2737,11 +2873,11 @@
       <c r="F20" s="17"/>
       <c r="G20" s="17"/>
     </row>
-    <row r="21" spans="1:7" s="19" customFormat="1">
+    <row r="21" spans="1:7" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="18">
         <v>8</v>
       </c>
-      <c r="B21" s="47" t="s">
+      <c r="B21" s="36" t="s">
         <v>64</v>
       </c>
       <c r="C21" s="15"/>
@@ -2750,11 +2886,11 @@
       <c r="F21" s="17"/>
       <c r="G21" s="17"/>
     </row>
-    <row r="22" spans="1:7" s="19" customFormat="1">
+    <row r="22" spans="1:7" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="18">
         <v>9</v>
       </c>
-      <c r="B22" s="47" t="s">
+      <c r="B22" s="36" t="s">
         <v>65</v>
       </c>
       <c r="C22" s="15"/>
@@ -2763,11 +2899,11 @@
       <c r="F22" s="17"/>
       <c r="G22" s="17"/>
     </row>
-    <row r="23" spans="1:7" s="19" customFormat="1">
+    <row r="23" spans="1:7" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="18">
         <v>10</v>
       </c>
-      <c r="B23" s="47" t="s">
+      <c r="B23" s="36" t="s">
         <v>66</v>
       </c>
       <c r="C23" s="15"/>
@@ -2776,11 +2912,11 @@
       <c r="F23" s="17"/>
       <c r="G23" s="17"/>
     </row>
-    <row r="24" spans="1:7" s="19" customFormat="1">
+    <row r="24" spans="1:7" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="18">
         <v>11</v>
       </c>
-      <c r="B24" s="47" t="s">
+      <c r="B24" s="36" t="s">
         <v>67</v>
       </c>
       <c r="C24" s="15"/>
@@ -2789,122 +2925,122 @@
       <c r="F24" s="17"/>
       <c r="G24" s="17"/>
     </row>
-    <row r="25" spans="1:7" s="19" customFormat="1">
+    <row r="25" spans="1:7" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="18">
         <v>12</v>
       </c>
-      <c r="B25" s="47" t="s">
+      <c r="B25" s="36" t="s">
         <v>68</v>
       </c>
-      <c r="C25" s="53"/>
+      <c r="C25" s="40"/>
       <c r="D25" s="17"/>
       <c r="E25" s="17"/>
       <c r="F25" s="17"/>
       <c r="G25" s="17"/>
     </row>
-    <row r="26" spans="1:7">
-      <c r="A26" s="51" t="s">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="53" t="s">
         <v>79</v>
       </c>
-      <c r="B26" s="52"/>
-      <c r="C26" s="52"/>
-      <c r="D26" s="45" t="s">
+      <c r="B26" s="54"/>
+      <c r="C26" s="54"/>
+      <c r="D26" s="34" t="s">
         <v>80</v>
       </c>
-      <c r="E26" s="45" t="s">
+      <c r="E26" s="34" t="s">
         <v>81</v>
       </c>
-      <c r="F26" s="45" t="s">
+      <c r="F26" s="34" t="s">
         <v>82</v>
       </c>
-      <c r="G26" s="45" t="s">
+      <c r="G26" s="34" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="27" spans="1:7">
-      <c r="A27" s="35"/>
-      <c r="B27" s="35"/>
-      <c r="C27" s="36"/>
-      <c r="D27" s="36"/>
-      <c r="E27" s="36"/>
-      <c r="F27" s="36"/>
-      <c r="G27" s="36"/>
-    </row>
-    <row r="28" spans="1:7" s="9" customFormat="1">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="26"/>
+      <c r="B27" s="26"/>
+      <c r="C27" s="27"/>
+      <c r="D27" s="27"/>
+      <c r="E27" s="27"/>
+      <c r="F27" s="27"/>
+      <c r="G27" s="27"/>
+    </row>
+    <row r="28" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B28" s="16"/>
       <c r="D28" s="9" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:7" s="9" customFormat="1">
+    <row r="29" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B29" s="16"/>
     </row>
-    <row r="30" spans="1:7">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="G30" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="31" spans="1:7" s="6" customFormat="1">
+    <row r="31" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="7" t="s">
         <v>22</v>
       </c>
       <c r="B31" s="7"/>
     </row>
-    <row r="32" spans="1:7">
-      <c r="A32" s="22" t="s">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" s="49" t="s">
         <v>23</v>
       </c>
-      <c r="B32" s="22"/>
-      <c r="C32" s="22"/>
-      <c r="D32" s="22"/>
-      <c r="E32" s="22"/>
-      <c r="F32" s="22"/>
-      <c r="G32" s="22"/>
-    </row>
-    <row r="33" spans="1:7">
+      <c r="B32" s="49"/>
+      <c r="C32" s="49"/>
+      <c r="D32" s="49"/>
+      <c r="E32" s="49"/>
+      <c r="F32" s="49"/>
+      <c r="G32" s="49"/>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
-      <c r="C33" s="22" t="s">
+      <c r="C33" s="49" t="s">
         <v>24</v>
       </c>
-      <c r="D33" s="22"/>
-      <c r="E33" s="22"/>
+      <c r="D33" s="49"/>
+      <c r="E33" s="49"/>
       <c r="F33" s="1"/>
       <c r="G33" s="1"/>
     </row>
-    <row r="34" spans="1:7">
-      <c r="C34" s="22" t="s">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C34" s="49" t="s">
         <v>25</v>
       </c>
-      <c r="D34" s="23"/>
-      <c r="E34" s="23"/>
-      <c r="F34" s="23"/>
-    </row>
-    <row r="36" spans="1:7">
-      <c r="A36" s="20" t="s">
+      <c r="D34" s="50"/>
+      <c r="E34" s="50"/>
+      <c r="F34" s="50"/>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" s="41" t="s">
         <v>1</v>
       </c>
       <c r="B36" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="C36" s="20" t="s">
+      <c r="C36" s="41" t="s">
         <v>2</v>
       </c>
-      <c r="D36" s="24" t="s">
+      <c r="D36" s="47" t="s">
         <v>3</v>
       </c>
-      <c r="E36" s="24"/>
-      <c r="F36" s="24" t="s">
+      <c r="E36" s="47"/>
+      <c r="F36" s="47" t="s">
         <v>4</v>
       </c>
-      <c r="G36" s="24"/>
-    </row>
-    <row r="37" spans="1:7">
-      <c r="A37" s="21"/>
+      <c r="G36" s="47"/>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" s="42"/>
       <c r="B37" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="C37" s="21"/>
+      <c r="C37" s="42"/>
       <c r="D37" s="17" t="s">
         <v>6</v>
       </c>
@@ -2918,7 +3054,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="38" spans="1:7">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="4"/>
       <c r="B38" s="3"/>
       <c r="C38" s="4"/>
@@ -2927,7 +3063,7 @@
       <c r="F38" s="4"/>
       <c r="G38" s="4"/>
     </row>
-    <row r="39" spans="1:7">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="4"/>
       <c r="B39" s="3"/>
       <c r="C39" s="4"/>
@@ -2936,7 +3072,7 @@
       <c r="F39" s="4"/>
       <c r="G39" s="4"/>
     </row>
-    <row r="40" spans="1:7">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="4"/>
       <c r="B40" s="3"/>
       <c r="C40" s="4"/>
@@ -2945,33 +3081,25 @@
       <c r="F40" s="4"/>
       <c r="G40" s="4"/>
     </row>
-    <row r="45" spans="1:7">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F45" s="6" t="s">
         <v>30</v>
       </c>
       <c r="G45" s="6"/>
     </row>
-    <row r="46" spans="1:7">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F46" s="6" t="s">
         <v>31</v>
       </c>
       <c r="G46" s="6"/>
     </row>
-    <row r="49" spans="6:6">
+    <row r="49" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F49" s="1" t="s">
         <v>32</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="A26:C26"/>
-    <mergeCell ref="A32:G32"/>
-    <mergeCell ref="C33:E33"/>
-    <mergeCell ref="C34:F34"/>
-    <mergeCell ref="A36:A37"/>
-    <mergeCell ref="C36:C37"/>
-    <mergeCell ref="D36:E36"/>
-    <mergeCell ref="F36:G36"/>
     <mergeCell ref="A2:G2"/>
     <mergeCell ref="A9:G9"/>
     <mergeCell ref="A10:M10"/>
@@ -2981,6 +3109,14 @@
     <mergeCell ref="C12:C13"/>
     <mergeCell ref="D12:E12"/>
     <mergeCell ref="F12:G12"/>
+    <mergeCell ref="A26:C26"/>
+    <mergeCell ref="A32:G32"/>
+    <mergeCell ref="C33:E33"/>
+    <mergeCell ref="C34:F34"/>
+    <mergeCell ref="A36:A37"/>
+    <mergeCell ref="C36:C37"/>
+    <mergeCell ref="D36:E36"/>
+    <mergeCell ref="F36:G36"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>